<commit_message>
Update product backlog and sprint backlog.
</commit_message>
<xml_diff>
--- a/sprint backlog project 4.xlsx
+++ b/sprint backlog project 4.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Sprint Backlog for project 4</t>
   </si>
@@ -41,15 +41,18 @@
     <t>1 hour</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>1-2 days</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>1-2 days</t>
-  </si>
-  <si>
     <t>Minigame1 (shooty snake)</t>
   </si>
   <si>
@@ -65,7 +68,7 @@
     <t>1 day</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>Display previous actions</t>
   </si>
   <si>
     <t>Alter code structure for testing</t>
@@ -87,6 +90,9 @@
   </si>
   <si>
     <t>Maintenance plan</t>
+  </si>
+  <si>
+    <t>2-3 days</t>
   </si>
 </sst>
 </file>
@@ -134,14 +140,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FF00FF66"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF66"/>
-        <bgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,10 +203,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,10 +287,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -338,25 +340,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -376,7 +372,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -396,37 +392,37 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>8</v>
@@ -434,40 +430,47 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Project4 sprint backlog
</commit_message>
<xml_diff>
--- a/sprint backlog project 4.xlsx
+++ b/sprint backlog project 4.xlsx
@@ -5,94 +5,129 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
-  <si>
-    <t>Sprint Backlog for project 4</t>
-  </si>
-  <si>
-    <t>Sub category</t>
-  </si>
-  <si>
-    <t>Name/Description</t>
-  </si>
-  <si>
-    <t>Estimated Time</t>
-  </si>
-  <si>
-    <t>Completed?</t>
-  </si>
-  <si>
-    <t>Main control interface</t>
-  </si>
-  <si>
-    <t>Menu graphics</t>
-  </si>
-  <si>
-    <t>1 hour</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>1-2 days</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Minigame1 (shooty snake)</t>
-  </si>
-  <si>
-    <t>Minigame 2 (pong)</t>
-  </si>
-  <si>
-    <t>Minigame 3 (nim)</t>
-  </si>
-  <si>
-    <t>Multiple difficullties</t>
-  </si>
-  <si>
-    <t>1 day</t>
-  </si>
-  <si>
-    <t>Display previous actions</t>
-  </si>
-  <si>
-    <t>Alter code structure for testing</t>
-  </si>
-  <si>
-    <t>1-2 hours</t>
-  </si>
-  <si>
-    <t>Test code for game mechanics</t>
-  </si>
-  <si>
-    <t>Documents</t>
-  </si>
-  <si>
-    <t>User's manual</t>
-  </si>
-  <si>
-    <t>Deployment plan</t>
-  </si>
-  <si>
-    <t>Maintenance plan</t>
-  </si>
-  <si>
-    <t>2-3 days</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+  <si>
+    <t xml:space="preserve">Sprint Backlog for project 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name/Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main control interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu graphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minigame1 (shooty snake)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve movement mechanics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add lone wolf mechanic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix off screen ball bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes (mostly)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add points and a leader board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minigame 2 (pong)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minigame 3 (nim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple difficullties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display previous actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter code structure for testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test code for game mechanics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User's manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deployment plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3 days</t>
   </si>
 </sst>
 </file>
@@ -100,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -287,19 +322,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,75 +388,93 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>8</v>
@@ -431,46 +483,70 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>21</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="4" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>